<commit_message>
[CEnemy] FSM(ft. function) 으로 IDLE, WALK 완
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. GameProject\DirectX11_Practice2D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1F2EF8-A027-4F70-B357-D4925750A5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B652C6F-E873-406D-9DBD-4462BE370B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="21036" windowHeight="12336" activeTab="1" xr2:uid="{968CEA55-0767-418E-8C7F-D2FC626DF758}"/>
+    <workbookView xWindow="4968" yWindow="0" windowWidth="16356" windowHeight="10692" activeTab="2" xr2:uid="{968CEA55-0767-418E-8C7F-D2FC626DF758}"/>
   </bookViews>
   <sheets>
     <sheet name="Skul" sheetId="2" r:id="rId1"/>
     <sheet name="Skill" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Enemy" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,16 +38,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="84">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ITEM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>등급</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -76,43 +72,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>요구뼈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>물리공격력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>물리데미지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마법공격력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>마법데미지</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>체력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공격속도</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이동속도</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>치명타</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>쿨다운속도</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -697,6 +661,22 @@
   </si>
   <si>
     <t>..\Bin\Resources\Skul\Player\GrimReaper_Effect\GateOfNether</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>병사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방어력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10, 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>248, =devide(1024/4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1136,7 +1116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C8398F3-D011-4647-AE44-4EA589985AAD}">
   <dimension ref="B3:O9"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
@@ -1154,7 +1134,7 @@
   <sheetData>
     <row r="3" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.4">
@@ -1162,63 +1142,63 @@
         <v>0</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="O4" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="K5">
         <v>10</v>
@@ -1227,27 +1207,27 @@
         <v>11</v>
       </c>
       <c r="N5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="104.4" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -1256,106 +1236,106 @@
         <v>44</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="H7" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="I7" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="M7">
         <v>22</v>
       </c>
       <c r="N7" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="H8" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="I8" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="M8">
         <v>33</v>
       </c>
       <c r="N8" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G9" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="H9" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="I9" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="M9">
         <v>44</v>
       </c>
       <c r="N9" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1368,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92D74111-5A06-453D-9354-EE86E8055134}">
   <dimension ref="B3:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1386,10 +1366,10 @@
   <sheetData>
     <row r="3" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="O3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.4">
@@ -1397,57 +1377,57 @@
         <v>0</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="J4" s="6" t="s">
+      <c r="M4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q4" s="6" t="s">
         <v>74</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="5" spans="2:17" ht="26.4" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -1468,30 +1448,30 @@
         <v>7</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="M5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="O5" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="P5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Q5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -1512,21 +1492,21 @@
         <v>5</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="M6" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E7">
         <v>10</v>
@@ -1544,21 +1524,21 @@
         <v>7</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="M7" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:17" ht="153.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E8">
         <v>10</v>
@@ -1576,21 +1556,21 @@
         <v>7</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="M8" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:17" ht="39.6" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -1608,21 +1588,21 @@
         <v>7</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="M9" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="2:17" ht="66" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E10">
         <v>10</v>
@@ -1640,21 +1620,21 @@
         <v>7</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="M10" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="2:17" ht="39.6" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E11">
         <v>10</v>
@@ -1672,10 +1652,10 @@
         <v>7</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="M11" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.4">
@@ -1689,84 +1669,73 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{030FEF9D-738D-422A-9878-E3C9EF4BAA2B}">
-  <dimension ref="B4:O9"/>
+  <dimension ref="B3:O5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" t="s">
+        <v>73</v>
+      </c>
+    </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" t="s">
-        <v>18</v>
+      <c r="L4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="D9" t="s">
-        <v>6</v>
+      <c r="C5" t="s">
+        <v>80</v>
+      </c>
+      <c r="K5" s="4"/>
+      <c r="N5" t="s">
+        <v>82</v>
+      </c>
+      <c r="O5" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>